<commit_message>
A couple months of changes
</commit_message>
<xml_diff>
--- a/TheRocket/data/variables.xlsx
+++ b/TheRocket/data/variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sk/Desktop/ICF /Shiller/github/TheRocket/TheRocket/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soshe\Documents\GitHub\TheRocket\TheRocket\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98A902E-44AF-F743-ACB4-E5854C3296C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB69666F-E676-44B4-8168-EA3D6A50A553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16940" activeTab="3" xr2:uid="{F762E12D-1FFF-2544-9934-8A4797DF9CC7}"/>
+    <workbookView xWindow="4050" yWindow="2580" windowWidth="21600" windowHeight="12670" activeTab="1" xr2:uid="{F762E12D-1FFF-2544-9934-8A4797DF9CC7}"/>
   </bookViews>
   <sheets>
     <sheet name="STRUCTURES" sheetId="5" r:id="rId1"/>
@@ -473,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -496,10 +496,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,7 +534,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
@@ -574,19 +570,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
@@ -829,7 +825,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -839,20 +835,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -924,7 +922,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -934,20 +932,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -1019,7 +1019,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1029,20 +1029,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -1114,7 +1116,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1124,20 +1126,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -1209,7 +1213,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1219,20 +1223,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -1304,7 +1310,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1314,20 +1320,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -1399,7 +1407,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1409,20 +1417,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -1494,7 +1504,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1504,20 +1514,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -1589,7 +1601,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1599,20 +1611,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -1684,7 +1698,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1694,20 +1708,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -1779,7 +1795,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1789,20 +1805,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -1874,7 +1892,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1884,20 +1902,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -1969,7 +1989,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1979,20 +1999,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -2064,7 +2086,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2074,20 +2096,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -2159,7 +2183,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2169,20 +2193,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -2254,7 +2280,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2264,20 +2290,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -2349,7 +2377,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2359,20 +2387,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -2444,7 +2474,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2454,20 +2484,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -2539,7 +2571,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2549,20 +2581,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -2634,7 +2668,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2644,20 +2678,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -2734,7 +2770,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2744,20 +2780,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -2829,7 +2867,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2839,20 +2877,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -2924,7 +2964,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2934,20 +2974,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -3019,7 +3061,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3029,20 +3071,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -3114,7 +3158,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3124,20 +3168,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -3209,7 +3255,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3219,20 +3265,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -3304,7 +3352,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3314,20 +3362,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -3404,7 +3454,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3414,20 +3464,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -3499,7 +3551,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3509,20 +3561,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -3594,7 +3648,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3604,20 +3658,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -3689,7 +3745,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3699,20 +3755,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -3789,7 +3847,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3799,20 +3857,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -3884,7 +3944,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3894,20 +3954,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -3979,7 +4041,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3989,20 +4051,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -4074,7 +4138,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4084,20 +4148,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -4169,7 +4235,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4179,20 +4245,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -4214,8 +4282,8 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>546100</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>203200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4264,7 +4332,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4274,20 +4342,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -4309,8 +4379,8 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>546100</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>203200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4359,7 +4429,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4369,20 +4439,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -4454,7 +4526,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4464,20 +4536,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -4549,7 +4623,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4559,20 +4633,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -4644,7 +4720,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4654,20 +4730,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -4739,7 +4817,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4749,20 +4827,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -4834,7 +4914,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4844,20 +4924,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -4929,7 +5011,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4939,20 +5021,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -5024,7 +5108,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5034,20 +5118,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -5119,7 +5205,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5129,20 +5215,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -5214,7 +5302,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5224,20 +5312,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -5309,7 +5399,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5319,20 +5409,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -5404,7 +5496,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5414,20 +5506,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -5499,7 +5593,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5509,20 +5603,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -5594,7 +5690,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5604,20 +5700,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -5689,7 +5787,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5699,20 +5797,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -5784,7 +5884,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5794,20 +5894,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -5879,7 +5981,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5889,20 +5991,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -5974,7 +6078,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5984,20 +6088,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -6069,7 +6175,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6079,20 +6185,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -6164,7 +6272,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6174,20 +6282,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -6259,7 +6369,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6269,20 +6379,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -6354,7 +6466,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6364,20 +6476,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -6449,7 +6563,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6459,20 +6573,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -6544,7 +6660,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6554,20 +6670,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -6639,7 +6757,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="0" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6649,20 +6767,22 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -6676,9 +6796,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6716,7 +6836,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6822,7 +6942,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6964,7 +7084,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6974,11 +7094,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F026DE90-7E8B-F545-B007-D15184FCF8D4}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView zoomScale="96" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="2"/>
@@ -6986,7 +7106,7 @@
     <col min="5" max="5" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>49</v>
       </c>
@@ -7003,7 +7123,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -7012,7 +7132,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -7023,7 +7143,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
@@ -7034,7 +7154,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -7045,7 +7165,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -7056,7 +7176,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -7067,7 +7187,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -7078,7 +7198,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -7087,7 +7207,7 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -7098,7 +7218,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -7109,7 +7229,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -7120,7 +7240,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -7131,7 +7251,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>7</v>
       </c>
@@ -7140,7 +7260,7 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -7151,7 +7271,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -7162,7 +7282,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>8</v>
       </c>
@@ -7171,7 +7291,7 @@
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -7179,7 +7299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -7190,7 +7310,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -7201,7 +7321,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -7212,7 +7332,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -7223,7 +7343,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>9</v>
       </c>
@@ -7232,7 +7352,7 @@
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -7244,7 +7364,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -7256,7 +7376,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -7731,16 +7851,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF97D7D-6D35-944A-BC59-497A90DC919B}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>49</v>
       </c>
@@ -7757,7 +7877,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>56</v>
       </c>
@@ -7766,7 +7886,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
@@ -7779,7 +7899,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -7792,7 +7912,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -7805,12 +7925,12 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="2">
-        <v>15</v>
+        <v>17.12</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>38</v>
@@ -7818,12 +7938,12 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="2">
-        <v>8</v>
+        <v>9.2469999999999999</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>39</v>
@@ -7831,12 +7951,12 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="2">
-        <v>5</v>
+        <v>3.02</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>39</v>
@@ -7844,7 +7964,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -8029,16 +8149,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07346C28-6DE3-DB46-A836-E40E364C1D11}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+    <sheetView zoomScale="95" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>49</v>
       </c>
@@ -8055,7 +8175,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>58</v>
       </c>
@@ -8064,12 +8184,12 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="2">
-        <v>14.4</v>
+        <v>18.059999999999999</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>38</v>
@@ -8077,7 +8197,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -8090,12 +8210,12 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="2">
-        <v>2.88</v>
+        <v>3.52</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>38</v>
@@ -8103,7 +8223,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -8116,21 +8236,21 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -8243,17 +8363,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CDFF95C-CAD7-8B45-9744-1F5C96B333C5}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="99" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>49</v>
       </c>
@@ -8270,7 +8390,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -8279,7 +8399,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -8289,7 +8409,7 @@
       <c r="C3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
@@ -8301,7 +8421,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -8313,7 +8433,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -8325,7 +8445,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -8338,7 +8458,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -8353,7 +8473,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -8365,7 +8485,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -8376,7 +8496,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>48</v>
       </c>
@@ -8387,7 +8507,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
@@ -8398,7 +8518,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>66</v>
       </c>
@@ -8412,7 +8532,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>67</v>
       </c>
@@ -8426,7 +8546,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
@@ -8437,7 +8557,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -8448,7 +8568,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>77</v>
       </c>
@@ -8457,7 +8577,7 @@
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>82</v>
       </c>
@@ -8471,7 +8591,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>83</v>
       </c>
@@ -8485,7 +8605,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>78</v>
       </c>
@@ -8494,7 +8614,7 @@
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>86</v>
       </c>
@@ -8508,7 +8628,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>79</v>
       </c>
@@ -8517,23 +8637,23 @@
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>80</v>
       </c>
@@ -8542,7 +8662,7 @@
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>90</v>
       </c>
@@ -8554,7 +8674,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>91</v>
       </c>
@@ -8569,7 +8689,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>92</v>
       </c>
@@ -8581,7 +8701,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -8596,7 +8716,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>93</v>
       </c>
@@ -8607,7 +8727,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>115</v>
       </c>
@@ -8616,7 +8736,7 @@
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
@@ -8631,7 +8751,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>104</v>
       </c>
@@ -8645,7 +8765,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>99</v>
       </c>
@@ -8659,7 +8779,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>100</v>
       </c>
@@ -8673,7 +8793,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>101</v>
       </c>
@@ -8687,7 +8807,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>81</v>
       </c>
@@ -8696,21 +8816,21 @@
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B38">
         <v>266</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" t="s">
         <v>111</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>103</v>
       </c>

</xml_diff>